<commit_message>
changes to the data sheet to add new data
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arpitsengar/IdeaProjects/Rest_Api_Framework/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FF7EEE-E38D-5C40-9229-A5535E81CCAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7007C9B8-EE17-D344-A195-5117945EE640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="460" windowWidth="24500" windowHeight="15000" activeTab="3" xr2:uid="{2334FA45-AC63-B044-8E66-AF4E051B16DE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="201">
   <si>
     <t>name</t>
   </si>
@@ -490,67 +490,154 @@
     <t>Natus maiores aliquid voluptates.</t>
   </si>
   <si>
-    <t>cus_Kv3Y6j083rX2bq</t>
-  </si>
-  <si>
-    <t>cus_Kv3YdUAFJ7lXq5</t>
-  </si>
-  <si>
-    <t>cus_Kv3Ytm6VAYfIya</t>
-  </si>
-  <si>
-    <t>cus_Kv3YNWL0dmw1Pj</t>
-  </si>
-  <si>
-    <t>cus_Kv3YHctEnei7LW</t>
-  </si>
-  <si>
-    <t>cus_Kv3YNy6MEBeKv4</t>
-  </si>
-  <si>
-    <t>cus_Kv3YncDwQfitwI</t>
-  </si>
-  <si>
-    <t>cus_Kv3YCNsnu4B2LV</t>
-  </si>
-  <si>
-    <t>cus_Kv3YZxNnOogDDP</t>
-  </si>
-  <si>
-    <t>cus_Kv3YLgk2lfy5g4</t>
-  </si>
-  <si>
-    <t>cus_Kv3Y2EvQQbPrtZ</t>
-  </si>
-  <si>
-    <t>cus_Kv3YdBXIaHEpGs</t>
-  </si>
-  <si>
-    <t>cus_Kv3YjPd7DI0K6x</t>
-  </si>
-  <si>
-    <t>cus_Kv3YPzlmCLYFfb</t>
-  </si>
-  <si>
-    <t>cus_Kv3YMVO5d0ooOl</t>
-  </si>
-  <si>
-    <t>cus_Kv3Ya4heB4TWT5</t>
-  </si>
-  <si>
-    <t>cus_Kv3YnmCFSmFS6c</t>
-  </si>
-  <si>
-    <t>cus_Kv3YTPpI07FcHo</t>
-  </si>
-  <si>
-    <t>cus_Kv3YaqQTJ1ZAkp</t>
-  </si>
-  <si>
-    <t>cus_Kv3Yadbo3fEtpg</t>
-  </si>
-  <si>
-    <t>cus_Kv3Y6xMTpeYkcf</t>
+    <t>cus_Kv3YAZpUxk7nBX</t>
+  </si>
+  <si>
+    <t>cus_Kv3Yj6sjAAuwsd</t>
+  </si>
+  <si>
+    <t>cus_Kv3Y0qTVOrYvhY</t>
+  </si>
+  <si>
+    <t>cus_Kv3YRJAn5ARQjp</t>
+  </si>
+  <si>
+    <t>cus_Kv3YdvFA4aOp5C</t>
+  </si>
+  <si>
+    <t>cus_Kv3YKC4NITLVzw</t>
+  </si>
+  <si>
+    <t>cus_Kv3YJHH005LtWZ</t>
+  </si>
+  <si>
+    <t>cus_Kv3YScFptrL85n</t>
+  </si>
+  <si>
+    <t>cus_Kv3YgFXgOniq1Z</t>
+  </si>
+  <si>
+    <t>cus_Kv3YmBMJws74x4</t>
+  </si>
+  <si>
+    <t>cus_Kv3YdhQ4XD17Nh</t>
+  </si>
+  <si>
+    <t>cus_Kv3YVf44eSRsVA</t>
+  </si>
+  <si>
+    <t>cus_Kv3YqxjpPoK7Bn</t>
+  </si>
+  <si>
+    <t>cus_Kv3YmyUsBPzHgQ</t>
+  </si>
+  <si>
+    <t>cus_Kv3YtMm6eQOin3</t>
+  </si>
+  <si>
+    <t>cus_Kv3YhqUukhBoit</t>
+  </si>
+  <si>
+    <t>cus_Kv3Y4uMUZdppAl</t>
+  </si>
+  <si>
+    <t>cus_Kv3YUIBSeZHp10</t>
+  </si>
+  <si>
+    <t>cus_Kv3YSVvTkyREvk</t>
+  </si>
+  <si>
+    <t>cus_Kv3YbR2pbfKvab</t>
+  </si>
+  <si>
+    <t>cus_Kv3YrFcLabBdar</t>
+  </si>
+  <si>
+    <t>cus_Kv3YWLCtW85X2Y</t>
+  </si>
+  <si>
+    <t>cus_Kv3YrEzvy3YgRP</t>
+  </si>
+  <si>
+    <t>cus_Kv3Y7JwQ4LMALT</t>
+  </si>
+  <si>
+    <t>cus_Kv3YAk4S69Ifee</t>
+  </si>
+  <si>
+    <t>cus_Kv3YqNAL7zSrkQ</t>
+  </si>
+  <si>
+    <t>cus_Kv3YWf5ahkCrGa</t>
+  </si>
+  <si>
+    <t>cus_Kv3YuD89KMvKWz</t>
+  </si>
+  <si>
+    <t>cus_Kv3YQYHCxSS5hs</t>
+  </si>
+  <si>
+    <t>cus_Kv3Y9qZyBll4Kn</t>
+  </si>
+  <si>
+    <t>cus_Kv3YYOW0c9t5p4</t>
+  </si>
+  <si>
+    <t>cus_Kv3YhYUEJinHoD</t>
+  </si>
+  <si>
+    <t>cus_Kv3XyI4k0v8uUn</t>
+  </si>
+  <si>
+    <t>cus_Kv3XnrzOJfZljq</t>
+  </si>
+  <si>
+    <t>cus_Kv3XDmjIyBmMjO</t>
+  </si>
+  <si>
+    <t>cus_Kv3XbB5jhWGe2M</t>
+  </si>
+  <si>
+    <t>cus_Kv3X60zEj4MBwp</t>
+  </si>
+  <si>
+    <t>cus_Kv3X39NWA8Ubfk</t>
+  </si>
+  <si>
+    <t>cus_Kv3Xz8RBr65Yrx</t>
+  </si>
+  <si>
+    <t>cus_Kv3XBze2VYr2nE</t>
+  </si>
+  <si>
+    <t>cus_Kv3XTji6ESoO4d</t>
+  </si>
+  <si>
+    <t>cus_Kv3XDAdGfeyeUR</t>
+  </si>
+  <si>
+    <t>cus_Kv3XgsO1MqgBuF</t>
+  </si>
+  <si>
+    <t>cus_Kv3XGlgLsZUuTV</t>
+  </si>
+  <si>
+    <t>cus_Kv3Xj195ajxsyY</t>
+  </si>
+  <si>
+    <t>cus_Kv3XhPav2vvMir</t>
+  </si>
+  <si>
+    <t>cus_Kv3XaRpjiTzUEL</t>
+  </si>
+  <si>
+    <t>cus_Kv3Xjv27Ut5Y1L</t>
+  </si>
+  <si>
+    <t>cus_Kv3Xckyn3mTVwf</t>
+  </si>
+  <si>
+    <t>cus_Kv3X8vwpwm8OdV</t>
   </si>
 </sst>
 </file>
@@ -1541,10 +1628,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF84709-DF56-BF48-992D-2FB427EF4323}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:A46"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1685,119 +1772,264 @@
         <v>129</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>125</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>126</v>
+      <c r="A25" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to the datasheet for check with jenkins and intergration of mail functionality
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arpitsengar/IdeaProjects/Rest_Api_Framework/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9439B0-7970-504C-83C9-A02F40598D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DFEA8F-B6B1-CA47-8F44-1F2E15BA82B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="460" windowWidth="24500" windowHeight="15000" activeTab="3" xr2:uid="{2334FA45-AC63-B044-8E66-AF4E051B16DE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="209">
   <si>
     <t>name</t>
   </si>
@@ -490,154 +490,178 @@
     <t>Natus maiores aliquid voluptates.</t>
   </si>
   <si>
-    <t>cus_Kv3YYOW0c9t5p4</t>
-  </si>
-  <si>
-    <t>cus_Kv3YhYUEJinHoD</t>
-  </si>
-  <si>
-    <t>cus_Kv3XyI4k0v8uUn</t>
-  </si>
-  <si>
-    <t>cus_Kv3XnrzOJfZljq</t>
-  </si>
-  <si>
-    <t>cus_Kv3XDmjIyBmMjO</t>
-  </si>
-  <si>
-    <t>cus_Kv3XbB5jhWGe2M</t>
-  </si>
-  <si>
-    <t>cus_Kv3X60zEj4MBwp</t>
-  </si>
-  <si>
-    <t>cus_Kv3X39NWA8Ubfk</t>
-  </si>
-  <si>
-    <t>cus_Kv3Xz8RBr65Yrx</t>
-  </si>
-  <si>
-    <t>cus_Kv3XBze2VYr2nE</t>
-  </si>
-  <si>
-    <t>cus_Kv3XTji6ESoO4d</t>
-  </si>
-  <si>
-    <t>cus_Kv3XDAdGfeyeUR</t>
-  </si>
-  <si>
-    <t>cus_Kv3XgsO1MqgBuF</t>
-  </si>
-  <si>
-    <t>cus_Kv3XGlgLsZUuTV</t>
-  </si>
-  <si>
-    <t>cus_Kv3Xj195ajxsyY</t>
-  </si>
-  <si>
-    <t>cus_Kv3XhPav2vvMir</t>
-  </si>
-  <si>
-    <t>cus_Kv3XaRpjiTzUEL</t>
-  </si>
-  <si>
-    <t>cus_Kv3Xjv27Ut5Y1L</t>
-  </si>
-  <si>
-    <t>cus_Kv3Xckyn3mTVwf</t>
-  </si>
-  <si>
-    <t>cus_Kv3X8vwpwm8OdV</t>
-  </si>
-  <si>
-    <t>cus_Kv3XOsEZTFmjDW</t>
-  </si>
-  <si>
-    <t>cus_Kv3XXdB1vGAo38</t>
-  </si>
-  <si>
-    <t>cus_Kv3X020eO8lguC</t>
-  </si>
-  <si>
-    <t>cus_Kv3XgOSFMBkpRh</t>
-  </si>
-  <si>
-    <t>cus_Kv3XD7mvwnktxU</t>
-  </si>
-  <si>
-    <t>cus_Kv3XRnnaf0jiP9</t>
-  </si>
-  <si>
-    <t>cus_Kv3Xtns0fScCt4</t>
-  </si>
-  <si>
-    <t>cus_Kv3XzDlmUMOz2P</t>
-  </si>
-  <si>
-    <t>cus_Kv3XwRKGaq5AZG</t>
-  </si>
-  <si>
-    <t>cus_Kv3Xg0y469rtXP</t>
-  </si>
-  <si>
-    <t>cus_Kv3X8lCj4ZlsJJ</t>
-  </si>
-  <si>
-    <t>cus_Kv3XWTseP4hkb6</t>
-  </si>
-  <si>
-    <t>cus_Kv3XaKdkIuTmAu</t>
-  </si>
-  <si>
-    <t>cus_Kv3XR8pASuv203</t>
-  </si>
-  <si>
-    <t>cus_Kv3PU7F3UvzCLW</t>
-  </si>
-  <si>
-    <t>cus_Kv3PQ4xeBzlevS</t>
-  </si>
-  <si>
-    <t>cus_Kv3PHj455pR49r</t>
-  </si>
-  <si>
-    <t>cus_Kv3PhbqE2WD89G</t>
-  </si>
-  <si>
-    <t>cus_Kv3Pq0lSMhDpBs</t>
-  </si>
-  <si>
-    <t>cus_Kv3PqN6r88hFcv</t>
-  </si>
-  <si>
-    <t>cus_Kv3PKOCL9q68rf</t>
-  </si>
-  <si>
-    <t>cus_Kv3PdNQrcKIaq9</t>
-  </si>
-  <si>
-    <t>cus_Kv3P01RdpJZtFe</t>
-  </si>
-  <si>
-    <t>cus_Kv3PS4M0ZmMXuZ</t>
-  </si>
-  <si>
-    <t>cus_Kv3Pg8Ughzltui</t>
-  </si>
-  <si>
-    <t>cus_Kv3PuHrHUDFOsK</t>
-  </si>
-  <si>
-    <t>cus_Kv3PrtRFBZ4j3K</t>
-  </si>
-  <si>
-    <t>cus_Kv3PjEKMVjD4eX</t>
-  </si>
-  <si>
-    <t>cus_Kv3PDAtiKEbjDq</t>
-  </si>
-  <si>
-    <t>cus_Kv3PYUrntTEKSr</t>
+    <t>cus_Kv3PKhR10oeVv8</t>
+  </si>
+  <si>
+    <t>cus_Kv3PFG1hgRZWjb</t>
+  </si>
+  <si>
+    <t>cus_Kv3PVe4TFfsmn1</t>
+  </si>
+  <si>
+    <t>cus_Kv3PBAyoMxQq0o</t>
+  </si>
+  <si>
+    <t>cus_Kv3PaJj4DnYMN5</t>
+  </si>
+  <si>
+    <t>cus_Kv3PSwErcjCMlm</t>
+  </si>
+  <si>
+    <t>cus_Kv3PNceLuZunTQ</t>
+  </si>
+  <si>
+    <t>cus_Kv3PhkC7XR8mZJ</t>
+  </si>
+  <si>
+    <t>cus_Kv3PsbsP7njhSP</t>
+  </si>
+  <si>
+    <t>cus_Kv3PV0lNudyNh0</t>
+  </si>
+  <si>
+    <t>cus_Kv3P6rTSOR4Rs2</t>
+  </si>
+  <si>
+    <t>cus_Kv3PqPLqSMMPUL</t>
+  </si>
+  <si>
+    <t>cus_Kv3PI8zu2CJVkT</t>
+  </si>
+  <si>
+    <t>cus_Kv3OzZlLr69Caq</t>
+  </si>
+  <si>
+    <t>cus_Kv3OLHTvvWS8fP</t>
+  </si>
+  <si>
+    <t>cus_Kv3ONbCYIbBmEd</t>
+  </si>
+  <si>
+    <t>cus_Kv3OWODvgmC3zn</t>
+  </si>
+  <si>
+    <t>cus_Kv3OOuXiVaJMbb</t>
+  </si>
+  <si>
+    <t>cus_Kv3O9eiZXUUj5X</t>
+  </si>
+  <si>
+    <t>cus_Kv3OAbnzNA4lvv</t>
+  </si>
+  <si>
+    <t>cus_Kv3Oc7sbKBB19j</t>
+  </si>
+  <si>
+    <t>cus_Kv3ODVudIqhtUk</t>
+  </si>
+  <si>
+    <t>cus_Kv3OyPLrN82gZM</t>
+  </si>
+  <si>
+    <t>cus_Kv3O9wlhwerkLy</t>
+  </si>
+  <si>
+    <t>cus_Kv3O8oXDmF9er1</t>
+  </si>
+  <si>
+    <t>cus_Kv3OYkh6rdGviM</t>
+  </si>
+  <si>
+    <t>cus_Kv3OpcSw4nRwYR</t>
+  </si>
+  <si>
+    <t>cus_Kv3OEUZtAkNf1o</t>
+  </si>
+  <si>
+    <t>cus_Kv3OAZXPwYPNjO</t>
+  </si>
+  <si>
+    <t>cus_Kv3OJTfbQY3Fxy</t>
+  </si>
+  <si>
+    <t>cus_Kv3Opqi4Uy7Uc1</t>
+  </si>
+  <si>
+    <t>cus_Kv3OPZUxy6Cszz</t>
+  </si>
+  <si>
+    <t>cus_Kv3O3o0IsQr3qH</t>
+  </si>
+  <si>
+    <t>cus_Kv3OWXQAUqEedz</t>
+  </si>
+  <si>
+    <t>cus_Kv3OBE59AKJ4UB</t>
+  </si>
+  <si>
+    <t>cus_Kv3OTW7Hu3Rf3s</t>
+  </si>
+  <si>
+    <t>cus_Kv3OHYq3WOKl14</t>
+  </si>
+  <si>
+    <t>cus_Kv3O0O1LTfoynI</t>
+  </si>
+  <si>
+    <t>cus_Kv3O6ckulx1QxD</t>
+  </si>
+  <si>
+    <t>cus_Kv3OaUog44fgIK</t>
+  </si>
+  <si>
+    <t>cus_Kv3OSuyNl4aZ8D</t>
+  </si>
+  <si>
+    <t>cus_Kv3OAFDXmPhCjC</t>
+  </si>
+  <si>
+    <t>cus_Kv3OKoiJlFNvyH</t>
+  </si>
+  <si>
+    <t>cus_Kv3NN05uR9X9zN</t>
+  </si>
+  <si>
+    <t>cus_Kv3NEGHcmOSdid</t>
+  </si>
+  <si>
+    <t>cus_Kv3NPF09fFXY32</t>
+  </si>
+  <si>
+    <t>cus_Kv3N2Ukbe1AXax</t>
+  </si>
+  <si>
+    <t>cus_Kv3NoPGPPz2Jlm</t>
+  </si>
+  <si>
+    <t>cus_Kv3NDr81Lqgiej</t>
+  </si>
+  <si>
+    <t>cus_Kv3NfYE6IOX4Pe</t>
+  </si>
+  <si>
+    <t>cus_Kv3NNARjxmimdQ</t>
+  </si>
+  <si>
+    <t>cus_Kv3Nk81SMdSLDL</t>
+  </si>
+  <si>
+    <t>cus_Kv3NDSOTqzfNhd</t>
+  </si>
+  <si>
+    <t>cus_Kv3Nwu4r8v76xV</t>
+  </si>
+  <si>
+    <t>cus_Kv3Nib3fHFBabm</t>
+  </si>
+  <si>
+    <t>cus_Kv3NLltNwlxwlr</t>
+  </si>
+  <si>
+    <t>cus_Kv3NpNnfkVwng2</t>
+  </si>
+  <si>
+    <t>cus_Kv3NwW2j0BdYwY</t>
   </si>
 </sst>
 </file>
@@ -1628,10 +1652,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF84709-DF56-BF48-992D-2FB427EF4323}">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:A48"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1784,252 +1808,292 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>151</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>152</v>
+        <v>182</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>153</v>
+        <v>183</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>154</v>
+        <v>184</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>155</v>
+        <v>185</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>156</v>
+        <v>186</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>157</v>
+        <v>187</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>158</v>
+        <v>188</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>159</v>
+        <v>189</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>160</v>
+        <v>190</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>161</v>
+        <v>191</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>162</v>
+        <v>192</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>163</v>
+        <v>193</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>164</v>
+        <v>194</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>165</v>
+        <v>195</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>166</v>
+        <v>196</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>167</v>
+        <v>197</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>168</v>
+        <v>198</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>169</v>
+        <v>199</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>170</v>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to the datasheet for check with jenkins and integration of mail functionality
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arpitsengar/IdeaProjects/Rest_Api_Framework/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DFEA8F-B6B1-CA47-8F44-1F2E15BA82B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9665D1-A48D-1A43-B8BE-F2BAE6EDE351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="460" windowWidth="24500" windowHeight="15000" activeTab="3" xr2:uid="{2334FA45-AC63-B044-8E66-AF4E051B16DE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="173">
   <si>
     <t>name</t>
   </si>
@@ -490,178 +490,70 @@
     <t>Natus maiores aliquid voluptates.</t>
   </si>
   <si>
-    <t>cus_Kv3PKhR10oeVv8</t>
-  </si>
-  <si>
-    <t>cus_Kv3PFG1hgRZWjb</t>
-  </si>
-  <si>
-    <t>cus_Kv3PVe4TFfsmn1</t>
-  </si>
-  <si>
-    <t>cus_Kv3PBAyoMxQq0o</t>
-  </si>
-  <si>
-    <t>cus_Kv3PaJj4DnYMN5</t>
-  </si>
-  <si>
-    <t>cus_Kv3PSwErcjCMlm</t>
-  </si>
-  <si>
-    <t>cus_Kv3PNceLuZunTQ</t>
-  </si>
-  <si>
-    <t>cus_Kv3PhkC7XR8mZJ</t>
-  </si>
-  <si>
-    <t>cus_Kv3PsbsP7njhSP</t>
-  </si>
-  <si>
-    <t>cus_Kv3PV0lNudyNh0</t>
-  </si>
-  <si>
-    <t>cus_Kv3P6rTSOR4Rs2</t>
-  </si>
-  <si>
-    <t>cus_Kv3PqPLqSMMPUL</t>
-  </si>
-  <si>
-    <t>cus_Kv3PI8zu2CJVkT</t>
-  </si>
-  <si>
-    <t>cus_Kv3OzZlLr69Caq</t>
-  </si>
-  <si>
-    <t>cus_Kv3OLHTvvWS8fP</t>
-  </si>
-  <si>
-    <t>cus_Kv3ONbCYIbBmEd</t>
-  </si>
-  <si>
-    <t>cus_Kv3OWODvgmC3zn</t>
-  </si>
-  <si>
-    <t>cus_Kv3OOuXiVaJMbb</t>
-  </si>
-  <si>
-    <t>cus_Kv3O9eiZXUUj5X</t>
-  </si>
-  <si>
-    <t>cus_Kv3OAbnzNA4lvv</t>
-  </si>
-  <si>
-    <t>cus_Kv3Oc7sbKBB19j</t>
-  </si>
-  <si>
-    <t>cus_Kv3ODVudIqhtUk</t>
-  </si>
-  <si>
-    <t>cus_Kv3OyPLrN82gZM</t>
-  </si>
-  <si>
-    <t>cus_Kv3O9wlhwerkLy</t>
-  </si>
-  <si>
-    <t>cus_Kv3O8oXDmF9er1</t>
-  </si>
-  <si>
-    <t>cus_Kv3OYkh6rdGviM</t>
-  </si>
-  <si>
-    <t>cus_Kv3OpcSw4nRwYR</t>
-  </si>
-  <si>
-    <t>cus_Kv3OEUZtAkNf1o</t>
-  </si>
-  <si>
-    <t>cus_Kv3OAZXPwYPNjO</t>
-  </si>
-  <si>
-    <t>cus_Kv3OJTfbQY3Fxy</t>
-  </si>
-  <si>
-    <t>cus_Kv3Opqi4Uy7Uc1</t>
-  </si>
-  <si>
-    <t>cus_Kv3OPZUxy6Cszz</t>
-  </si>
-  <si>
-    <t>cus_Kv3O3o0IsQr3qH</t>
-  </si>
-  <si>
-    <t>cus_Kv3OWXQAUqEedz</t>
-  </si>
-  <si>
-    <t>cus_Kv3OBE59AKJ4UB</t>
-  </si>
-  <si>
-    <t>cus_Kv3OTW7Hu3Rf3s</t>
-  </si>
-  <si>
-    <t>cus_Kv3OHYq3WOKl14</t>
-  </si>
-  <si>
-    <t>cus_Kv3O0O1LTfoynI</t>
-  </si>
-  <si>
-    <t>cus_Kv3O6ckulx1QxD</t>
-  </si>
-  <si>
-    <t>cus_Kv3OaUog44fgIK</t>
-  </si>
-  <si>
-    <t>cus_Kv3OSuyNl4aZ8D</t>
-  </si>
-  <si>
-    <t>cus_Kv3OAFDXmPhCjC</t>
-  </si>
-  <si>
-    <t>cus_Kv3OKoiJlFNvyH</t>
-  </si>
-  <si>
-    <t>cus_Kv3NN05uR9X9zN</t>
-  </si>
-  <si>
-    <t>cus_Kv3NEGHcmOSdid</t>
-  </si>
-  <si>
-    <t>cus_Kv3NPF09fFXY32</t>
-  </si>
-  <si>
-    <t>cus_Kv3N2Ukbe1AXax</t>
-  </si>
-  <si>
-    <t>cus_Kv3NoPGPPz2Jlm</t>
-  </si>
-  <si>
-    <t>cus_Kv3NDr81Lqgiej</t>
-  </si>
-  <si>
-    <t>cus_Kv3NfYE6IOX4Pe</t>
-  </si>
-  <si>
-    <t>cus_Kv3NNARjxmimdQ</t>
-  </si>
-  <si>
-    <t>cus_Kv3Nk81SMdSLDL</t>
-  </si>
-  <si>
-    <t>cus_Kv3NDSOTqzfNhd</t>
-  </si>
-  <si>
-    <t>cus_Kv3Nwu4r8v76xV</t>
-  </si>
-  <si>
-    <t>cus_Kv3Nib3fHFBabm</t>
-  </si>
-  <si>
-    <t>cus_Kv3NLltNwlxwlr</t>
-  </si>
-  <si>
-    <t>cus_Kv3NpNnfkVwng2</t>
-  </si>
-  <si>
-    <t>cus_Kv3NwW2j0BdYwY</t>
+    <t>cus_Kv3NNXOk2nWmh3</t>
+  </si>
+  <si>
+    <t>cus_Kv3NM8lN8vTSRd</t>
+  </si>
+  <si>
+    <t>cus_Kv3NKvf9UkFTwJ</t>
+  </si>
+  <si>
+    <t>cus_Kv3NsPc8mUAUHg</t>
+  </si>
+  <si>
+    <t>cus_Kv3NLaOxqFK95z</t>
+  </si>
+  <si>
+    <t>cus_Kv3NGBoZg9yZcZ</t>
+  </si>
+  <si>
+    <t>cus_Kv3N22I2BOFbuv</t>
+  </si>
+  <si>
+    <t>cus_Kv3NLfgvNOINlb</t>
+  </si>
+  <si>
+    <t>cus_Kv3NfUhd7XfnxZ</t>
+  </si>
+  <si>
+    <t>cus_Kv3N6tQI3FzQWF</t>
+  </si>
+  <si>
+    <t>cus_Kv3NPnn1hm5Jx8</t>
+  </si>
+  <si>
+    <t>cus_Kv3NDeLsrnPa8k</t>
+  </si>
+  <si>
+    <t>cus_Kv3NOirrfpE4VI</t>
+  </si>
+  <si>
+    <t>cus_Kv3NMP3KqwNl0k</t>
+  </si>
+  <si>
+    <t>cus_Kv3NKmz1AtGURh</t>
+  </si>
+  <si>
+    <t>cus_Kv3NoziMXiNZll</t>
+  </si>
+  <si>
+    <t>cus_Kv3N2rFCyLLjWj</t>
+  </si>
+  <si>
+    <t>cus_Kv3Njxv0unpFTw</t>
+  </si>
+  <si>
+    <t>cus_Kv3Np43XgxP5w8</t>
+  </si>
+  <si>
+    <t>cus_Kv3NWrwrreXumo</t>
+  </si>
+  <si>
+    <t>getCustomerDetails</t>
+  </si>
+  <si>
+    <t>cus_Kv3kMI4KlpKN94</t>
   </si>
 </sst>
 </file>
@@ -1652,10 +1544,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF84709-DF56-BF48-992D-2FB427EF4323}">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:A76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1906,194 +1798,19 @@
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Editing of the files to remove the extent report statement
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arpitsengar/IdeaProjects/Rest_Api_Framework/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9665D1-A48D-1A43-B8BE-F2BAE6EDE351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80C9EA1-E67C-EF41-9839-0D25693DF631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="460" windowWidth="24500" windowHeight="15000" activeTab="3" xr2:uid="{2334FA45-AC63-B044-8E66-AF4E051B16DE}"/>
   </bookViews>
@@ -553,20 +553,25 @@
     <t>getCustomerDetails</t>
   </si>
   <si>
-    <t>cus_Kv3kMI4KlpKN94</t>
+    <t>cus_L3llWW1kbMZRec</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Source Sans Pro"/>
     </font>
   </fonts>
   <fills count="4">
@@ -616,12 +621,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1546,8 +1552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF84709-DF56-BF48-992D-2FB427EF4323}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1808,8 +1814,8 @@
         <v>126</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="42" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>172</v>
       </c>
     </row>

</xml_diff>